<commit_message>
Updated Burndown Chart Sprint 2 October 8th
</commit_message>
<xml_diff>
--- a/Architecture Patterns, Diagrams and Charts/BurndownChart-Grp004 Sprint2.xlsx
+++ b/Architecture Patterns, Diagrams and Charts/BurndownChart-Grp004 Sprint2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\Periscope\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{26C12303-E33E-4200-ABFB-99FCC9DF127C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E074EC-D8F8-49DF-8A18-DAB592F7B3E6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1087,6 +1087,21 @@
                 <c:pt idx="4">
                   <c:v>38</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>25</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2744,8 +2759,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2883,30 +2898,45 @@
         <v>15</v>
       </c>
       <c r="B18" s="4"/>
+      <c r="C18" s="1">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>14</v>
       </c>
       <c r="B19" s="4"/>
+      <c r="C19" s="1">
+        <v>33</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>13</v>
       </c>
       <c r="B20" s="4"/>
+      <c r="C20" s="1">
+        <v>31</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>12</v>
       </c>
       <c r="B21" s="4"/>
+      <c r="C21" s="1">
+        <v>28</v>
+      </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>11</v>
       </c>
       <c r="B22" s="4"/>
+      <c r="C22" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="1">

</xml_diff>

<commit_message>
Burndown Chart Updated for October 15th
</commit_message>
<xml_diff>
--- a/Architecture Patterns, Diagrams and Charts/BurndownChart-Grp004 Sprint2.xlsx
+++ b/Architecture Patterns, Diagrams and Charts/BurndownChart-Grp004 Sprint2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\Periscope\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43E074EC-D8F8-49DF-8A18-DAB592F7B3E6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{157D7225-9F47-41AF-A409-63F6EA967CDE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Burn down chart" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -949,7 +950,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1073,34 +1074,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>44</c:v>
+                  <c:v>58</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>43</c:v>
+                  <c:v>57</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>41</c:v>
+                  <c:v>55</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>38</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33</c:v>
+                  <c:v>47</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>31</c:v>
+                  <c:v>45</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>28</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="12">
                   <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2759,8 +2775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2851,10 +2867,10 @@
         <v>20</v>
       </c>
       <c r="B13" s="1">
-        <v>44</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2863,7 +2879,7 @@
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="1">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -2872,7 +2888,7 @@
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="1">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -2881,7 +2897,7 @@
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="1">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2890,7 +2906,7 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="1">
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2899,7 +2915,7 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="1">
-        <v>36</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2908,7 +2924,7 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="1">
-        <v>33</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2917,7 +2933,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="1">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2926,7 +2942,7 @@
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="1">
-        <v>28</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2935,7 +2951,7 @@
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="1">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2943,30 +2959,45 @@
         <v>10</v>
       </c>
       <c r="B23" s="4"/>
+      <c r="C23" s="1">
+        <v>34</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>9</v>
       </c>
       <c r="B24" s="4"/>
+      <c r="C24" s="1">
+        <v>29</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>8</v>
       </c>
       <c r="B25" s="4"/>
+      <c r="C25" s="1">
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>7</v>
       </c>
       <c r="B26" s="4"/>
+      <c r="C26" s="1">
+        <v>22</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>6</v>
       </c>
       <c r="B27" s="4"/>
+      <c r="C27" s="1">
+        <v>18</v>
+      </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="1">

</xml_diff>

<commit_message>
Finished Sprint 2 Burndown and Release Chart
</commit_message>
<xml_diff>
--- a/Architecture Patterns, Diagrams and Charts/BurndownChart-Grp004 Sprint2.xlsx
+++ b/Architecture Patterns, Diagrams and Charts/BurndownChart-Grp004 Sprint2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\Periscope\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{157D7225-9F47-41AF-A409-63F6EA967CDE}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F66DE6-9A4E-4091-A957-E367B063DB71}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Burn down chart" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -302,10 +301,17 @@
           </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>'Burn down chart'!$A$3:$A$7</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burn down chart'!$A$3:$A$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Burn down chart'!$A$3:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -314,27 +320,25 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Burn down chart'!$B$3:$B$7</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burn down chart'!$B$3:$B$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Burn down chart'!$B$3:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -386,10 +390,17 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Burn down chart'!$A$3:$A$7</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burn down chart'!$A$3:$A$7</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Burn down chart'!$A$3:$A$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -410,6 +421,13 @@
           </c:cat>
           <c:val>
             <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>'Burn down chart'!$C$3:$C$5</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
               <c:f>'Burn down chart'!$C$3:$C$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -419,6 +437,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1118,6 +1139,24 @@
                 <c:pt idx="14">
                   <c:v>18</c:v>
                 </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -2775,8 +2814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2829,6 +2868,9 @@
         <v>2</v>
       </c>
       <c r="B5" s="3"/>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -3004,30 +3046,45 @@
         <v>5</v>
       </c>
       <c r="B28" s="4"/>
+      <c r="C28" s="1">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>4</v>
       </c>
       <c r="B29" s="4"/>
+      <c r="C29" s="1">
+        <v>10</v>
+      </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>3</v>
       </c>
       <c r="B30" s="4"/>
+      <c r="C30" s="1">
+        <v>6</v>
+      </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>2</v>
       </c>
       <c r="B31" s="4"/>
+      <c r="C31" s="1">
+        <v>3</v>
+      </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>1</v>
       </c>
       <c r="B32" s="4"/>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -3035,6 +3092,9 @@
         <v>0</v>
       </c>
       <c r="B33" s="1">
+        <v>0</v>
+      </c>
+      <c r="C33" s="1">
         <v>0</v>
       </c>
       <c r="D33" s="2"/>

</xml_diff>

<commit_message>
burndown updated and complete
</commit_message>
<xml_diff>
--- a/Architecture Patterns, Diagrams and Charts/BurndownChart-Grp004 Sprint2.xlsx
+++ b/Architecture Patterns, Diagrams and Charts/BurndownChart-Grp004 Sprint2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matt Da Bomb\Desktop\Periscope\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ifb299perfectbalance\Architecture Patterns, Diagrams and Charts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F66DE6-9A4E-4091-A957-E367B063DB71}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3FA565F-8391-47B9-ACEF-D5714209FE69}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn down chart" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Sprint Days Remaining</t>
   </si>
@@ -41,9 +41,6 @@
   </si>
   <si>
     <t>Release Burndown</t>
-  </si>
-  <si>
-    <t>ALSO DO A SPRINT 2 BURNDOWN AS WELL</t>
   </si>
   <si>
     <t>Sprint 2 Burndown</t>
@@ -338,7 +335,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -433,10 +430,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -971,7 +968,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="20">
                   <c:v>0</c:v>
@@ -1095,28 +1092,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="21"/>
                 <c:pt idx="0">
-                  <c:v>58</c:v>
+                  <c:v>77</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>55</c:v>
+                  <c:v>71</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>52</c:v>
                 </c:pt>
-                <c:pt idx="5">
-                  <c:v>50</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>47</c:v>
-                </c:pt>
                 <c:pt idx="7">
-                  <c:v>45</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>42</c:v>
@@ -2814,8 +2811,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2848,10 +2845,10 @@
         <v>0</v>
       </c>
       <c r="B3" s="1">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C3" s="1">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2860,7 +2857,7 @@
       </c>
       <c r="B4" s="3"/>
       <c r="C4" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2888,7 +2885,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2909,10 +2906,10 @@
         <v>20</v>
       </c>
       <c r="B13" s="1">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C13" s="1">
-        <v>58</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -2921,7 +2918,7 @@
       </c>
       <c r="B14" s="4"/>
       <c r="C14" s="1">
-        <v>57</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -2930,7 +2927,7 @@
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="1">
-        <v>55</v>
+        <v>71</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -2939,7 +2936,7 @@
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="1">
-        <v>54</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2948,7 +2945,7 @@
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="1">
-        <v>52</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2957,7 +2954,7 @@
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="1">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2966,7 +2963,7 @@
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="1">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2975,7 +2972,7 @@
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="1">
-        <v>45</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3106,9 +3103,6 @@
       <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>